<commit_message>
scafolding de los dashboards
</commit_message>
<xml_diff>
--- a/entidades.xlsx
+++ b/entidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>teams</t>
   </si>
@@ -102,6 +102,39 @@
   </si>
   <si>
     <t>organizer{id, etc…}</t>
+  </si>
+  <si>
+    <t>add team to tournaments</t>
+  </si>
+  <si>
+    <t>tourId</t>
+  </si>
+  <si>
+    <t>teamName</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>friends[]</t>
+  </si>
+  <si>
+    <t>myTournaments[]</t>
+  </si>
+  <si>
+    <t>idTournaments</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>tournamentName</t>
+  </si>
+  <si>
+    <t>tournament</t>
+  </si>
+  <si>
+    <t>idTeam</t>
   </si>
 </sst>
 </file>
@@ -436,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -455,150 +488,177 @@
     <col min="11" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="F9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A26" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A31" s="2" t="s">
-        <v>13</v>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.4">

</xml_diff>